<commit_message>
cabeçalho em todas as folhas relatorio
</commit_message>
<xml_diff>
--- a/src/pause-web/src/main/resources/QA360Relatorio.xlsx
+++ b/src/pause-web/src/main/resources/QA360Relatorio.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="QA360" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'QA360'!$1:$5</definedName>
+  </definedNames>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
@@ -179,20 +182,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -250,8 +253,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>97316</xdr:rowOff>
     </xdr:to>
@@ -592,10 +595,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:AA29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y1" sqref="Y1:Y1048576"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,96 +625,96 @@
     <col min="17" max="17" width="3" customWidth="1"/>
     <col min="18" max="18" width="9" customWidth="1"/>
     <col min="19" max="19" width="3" customWidth="1"/>
-    <col min="21" max="21" width="7.140625" style="13" customWidth="1"/>
-    <col min="22" max="23" width="9.140625" style="13"/>
-    <col min="24" max="24" width="7.140625" style="13" customWidth="1"/>
-    <col min="25" max="25" width="8.28515625" style="13" customWidth="1"/>
+    <col min="21" max="21" width="7.140625" style="8" customWidth="1"/>
+    <col min="22" max="23" width="9.140625" style="8"/>
+    <col min="24" max="24" width="7.140625" style="8" customWidth="1"/>
+    <col min="25" max="25" width="8.28515625" style="8" customWidth="1"/>
     <col min="27" max="27" width="2.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="36" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="12" t="s">
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="9" t="s">
+      <c r="F2" s="14"/>
+      <c r="G2" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
       <c r="R2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="S2" s="8" t="s">
+      <c r="S2" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
+      <c r="T2" s="15"/>
+      <c r="U2" s="15"/>
+      <c r="V2" s="15"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="R3" s="8" t="s">
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="R3" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
+      <c r="S3" s="15"/>
+      <c r="T3" s="15"/>
+      <c r="U3" s="15"/>
+      <c r="V3" s="15"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -771,19 +777,19 @@
       <c r="T5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="U5" s="14" t="s">
+      <c r="U5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="V5" s="14" t="s">
+      <c r="V5" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="W5" s="14" t="s">
+      <c r="W5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="X5" s="14" t="s">
+      <c r="X5" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="Y5" s="14" t="s">
+      <c r="Y5" s="9" t="s">
         <v>19</v>
       </c>
       <c r="Z5" s="4" t="s">
@@ -878,11 +884,11 @@
       <c r="R9" s="5"/>
       <c r="S9" s="6"/>
       <c r="T9" s="6"/>
-      <c r="U9" s="15"/>
-      <c r="V9" s="15"/>
-      <c r="W9" s="15"/>
-      <c r="X9" s="15"/>
-      <c r="Y9" s="15"/>
+      <c r="U9" s="10"/>
+      <c r="V9" s="10"/>
+      <c r="W9" s="10"/>
+      <c r="X9" s="10"/>
+      <c r="Y9" s="10"/>
       <c r="Z9" s="6"/>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
@@ -1103,8 +1109,8 @@
     <mergeCell ref="B3:I3"/>
     <mergeCell ref="R3:V3"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.34166666666666667" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="80" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;LLegenda : Origem Marcação: M- Manual / E- Eletrônico / SA = Sobre Aviso (Plantão); SA = Sobre Aviso sem Acionamento / ST = Sobre Aviso Trabalhado / TP = Tipo do Ponto</oddFooter>
   </headerFooter>

</xml_diff>